<commit_message>
Signed-off-by: sarah <2818724775@qq.com> 日常练习
</commit_message>
<xml_diff>
--- a/LogManagement/doc/学习记录.xlsx
+++ b/LogManagement/doc/学习记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="8484" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="23040" windowHeight="9347" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="娄梦月" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>日期时间</t>
   </si>
@@ -42,6 +42,42 @@
   </si>
   <si>
     <t>数据库的配置及简单操作</t>
+  </si>
+  <si>
+    <t>2019/4/4 9:00--11:00</t>
+  </si>
+  <si>
+    <t>单元测试</t>
+  </si>
+  <si>
+    <t>2019/4/8 9:00--11:00</t>
+  </si>
+  <si>
+    <t>把表格读取到数据库里</t>
+  </si>
+  <si>
+    <t>2019/4/15 9:00--11:00</t>
+  </si>
+  <si>
+    <t>Dao模块的建立</t>
+  </si>
+  <si>
+    <t>2019/4/16 9:00--11:00</t>
+  </si>
+  <si>
+    <t>添加hibernate-entitymanager</t>
+  </si>
+  <si>
+    <t>2019/4/17 9:00--11:00</t>
+  </si>
+  <si>
+    <t>模拟上课内容建立device实体类</t>
+  </si>
+  <si>
+    <t>2019/4/21 9:00--11:00</t>
+  </si>
+  <si>
+    <t>学习maven命令</t>
   </si>
   <si>
     <t>2019/4/15 8:30--10:30</t>
@@ -261,10 +297,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -276,6 +312,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -283,7 +326,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,6 +355,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -306,7 +425,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,54 +433,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -380,44 +454,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -428,187 +464,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,6 +658,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -629,6 +680,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,21 +717,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -676,16 +727,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -704,21 +755,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -727,10 +763,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -739,133 +775,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1253,13 +1289,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90740740740741" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.90740740740741" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="29.9074074074074" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.4537037037037" style="1" customWidth="1"/>
@@ -1287,6 +1323,54 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1328,10 +1412,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1376,71 +1460,71 @@
         <v>43561</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1491,7 +1575,7 @@
   <sheetPr/>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1519,66 +1603,66 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1620,18 +1704,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1673,87 +1757,87 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>